<commit_message>
Updates for oter-NLP Excel reports after proper attribute key sorting
</commit_message>
<xml_diff>
--- a/docs/influence/auto/anger/gw_full_nlp_n5-25_oter_anger.xlsx
+++ b/docs/influence/auto/anger/gw_full_nlp_n5-25_oter_anger.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/cat/Users/dend/prog/say_sila/docs/influence/auto/anger/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2D4C04-A78D-0648-ABAF-0535258398A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4446E2F5-B901-2D41-935A-123E60BD96DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60180" yWindow="8160" windowWidth="32900" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="460" windowWidth="32480" windowHeight="20540"/>
   </bookViews>
   <sheets>
     <sheet name="gw_full_nlp_n5-25_oter_anger" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -938,11 +938,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD11"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1032,13 +1032,13 @@
         <v>25</v>
       </c>
       <c r="E2">
-        <v>-0.43936799999999998</v>
+        <v>-0.44717000000000001</v>
       </c>
       <c r="F2">
         <v>39</v>
       </c>
       <c r="W2">
-        <v>0.15673400000000001</v>
+        <v>0.15631500000000001</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
@@ -1055,13 +1055,16 @@
         <v>25</v>
       </c>
       <c r="E3">
-        <v>-0.43450299999999997</v>
+        <v>-8.3267999999999995E-2</v>
       </c>
       <c r="F3">
         <v>39</v>
       </c>
+      <c r="T3">
+        <v>-7.1578000000000003E-2</v>
+      </c>
       <c r="W3">
-        <v>0.15853999999999999</v>
+        <v>0.171656</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
@@ -1078,28 +1081,28 @@
         <v>25</v>
       </c>
       <c r="E4">
-        <v>0.661991</v>
+        <v>0.64805699999999999</v>
       </c>
       <c r="F4">
         <v>39</v>
       </c>
       <c r="H4">
-        <v>0.20839199999999999</v>
+        <v>0.209924</v>
       </c>
       <c r="J4">
-        <v>0.237627</v>
+        <v>0.22464500000000001</v>
       </c>
       <c r="K4">
-        <v>0.11742900000000001</v>
+        <v>0.111431</v>
       </c>
       <c r="O4">
-        <v>-6.0257999999999999E-2</v>
+        <v>-6.1193999999999998E-2</v>
       </c>
       <c r="Q4">
-        <v>5.8241000000000001E-2</v>
+        <v>5.6621999999999999E-2</v>
       </c>
       <c r="W4">
-        <v>-2.5724E-2</v>
+        <v>-1.8796E-2</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
@@ -1116,25 +1119,22 @@
         <v>25</v>
       </c>
       <c r="E5">
-        <v>0.39065800000000001</v>
+        <v>0.62830399999999997</v>
       </c>
       <c r="F5">
         <v>39</v>
       </c>
-      <c r="G5">
-        <v>0.54472799999999999</v>
+      <c r="H5">
+        <v>0.29997800000000002</v>
       </c>
       <c r="K5">
-        <v>0.193831</v>
-      </c>
-      <c r="T5">
-        <v>-8.5061999999999999E-2</v>
-      </c>
-      <c r="U5">
-        <v>0.120494</v>
+        <v>0.41192600000000001</v>
+      </c>
+      <c r="M5">
+        <v>-0.42371999999999999</v>
       </c>
       <c r="W5">
-        <v>2.7079999999999999E-3</v>
+        <v>5.2429000000000003E-2</v>
       </c>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1151,22 +1151,25 @@
         <v>25</v>
       </c>
       <c r="E6" s="1">
-        <v>0.71029799999999998</v>
+        <v>0.73074499999999998</v>
       </c>
       <c r="F6" s="1">
         <v>39</v>
       </c>
       <c r="G6" s="1">
-        <v>0.54094500000000001</v>
+        <v>0.360095</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.134348</v>
       </c>
       <c r="K6" s="1">
-        <v>0.24978</v>
+        <v>0.247201</v>
       </c>
       <c r="L6" s="1">
-        <v>-0.122673</v>
+        <v>-0.13377700000000001</v>
       </c>
       <c r="W6" s="1">
-        <v>2.9666999999999999E-2</v>
+        <v>2.9527999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
@@ -1183,72 +1186,75 @@
         <v>25</v>
       </c>
       <c r="E7">
-        <v>0.68787500000000001</v>
+        <v>0.67978000000000005</v>
       </c>
       <c r="F7">
         <v>39</v>
       </c>
       <c r="G7">
-        <v>0.35205199999999998</v>
+        <v>0.29917100000000002</v>
       </c>
       <c r="H7">
-        <v>0.122749</v>
+        <v>0.15281400000000001</v>
       </c>
       <c r="K7">
-        <v>0.21865999999999999</v>
-      </c>
-      <c r="L7">
-        <v>-9.9048999999999998E-2</v>
+        <v>0.27542100000000003</v>
+      </c>
+      <c r="M7">
+        <v>-0.25108900000000001</v>
       </c>
       <c r="O7">
-        <v>-4.2908000000000002E-2</v>
-      </c>
-      <c r="Q7">
-        <v>6.1799E-2</v>
+        <v>-4.1363999999999998E-2</v>
       </c>
       <c r="S7">
-        <v>-6.7932999999999993E-2</v>
+        <v>-5.4470999999999999E-2</v>
       </c>
       <c r="U7">
-        <v>8.5624000000000006E-2</v>
+        <v>9.1841000000000006E-2</v>
       </c>
       <c r="W7">
-        <v>3.5716999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+        <v>4.8723000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.760849</v>
-      </c>
-      <c r="F8" s="1">
-        <v>39</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.31526900000000002</v>
-      </c>
-      <c r="H8" s="1">
-        <v>8.8838E-2</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0.21295800000000001</v>
-      </c>
-      <c r="L8" s="1">
-        <v>-0.100078</v>
-      </c>
-      <c r="W8" s="1">
-        <v>5.4672999999999999E-2</v>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>0.65213399999999999</v>
+      </c>
+      <c r="F8">
+        <v>39</v>
+      </c>
+      <c r="G8">
+        <v>0.31885599999999997</v>
+      </c>
+      <c r="H8">
+        <v>8.1597000000000003E-2</v>
+      </c>
+      <c r="K8">
+        <v>0.18739</v>
+      </c>
+      <c r="L8">
+        <v>-9.9285999999999999E-2</v>
+      </c>
+      <c r="T8">
+        <v>-6.9281999999999996E-2</v>
+      </c>
+      <c r="U8">
+        <v>9.3186000000000005E-2</v>
+      </c>
+      <c r="W8">
+        <v>6.2462999999999998E-2</v>
       </c>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1265,112 +1271,124 @@
         <v>25</v>
       </c>
       <c r="E9" s="1">
-        <v>0.760154</v>
+        <v>0.77123200000000003</v>
       </c>
       <c r="F9" s="1">
         <v>39</v>
       </c>
       <c r="G9" s="1">
-        <v>0.28167799999999998</v>
+        <v>0.25820300000000002</v>
       </c>
       <c r="H9" s="1">
-        <v>7.3218000000000005E-2</v>
+        <v>8.6004999999999998E-2</v>
       </c>
       <c r="K9" s="1">
-        <v>0.22209300000000001</v>
+        <v>0.22355</v>
       </c>
       <c r="L9" s="1">
-        <v>-9.4343999999999997E-2</v>
+        <v>-0.10020900000000001</v>
       </c>
       <c r="W9" s="1">
-        <v>6.4071000000000003E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+        <v>6.6115999999999994E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>13</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.72134399999999999</v>
-      </c>
-      <c r="F10" s="1">
-        <v>39</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.30836200000000002</v>
-      </c>
-      <c r="K10" s="1">
-        <v>0.12705</v>
-      </c>
-      <c r="W10" s="1">
-        <v>7.1093000000000003E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <v>0.55827800000000005</v>
+      </c>
+      <c r="F10">
+        <v>39</v>
+      </c>
+      <c r="G10">
+        <v>0.30663200000000002</v>
+      </c>
+      <c r="K10">
+        <v>0.104533</v>
+      </c>
+      <c r="T10">
+        <v>-5.2776000000000003E-2</v>
+      </c>
+      <c r="U10">
+        <v>7.3405999999999999E-2</v>
+      </c>
+      <c r="W10">
+        <v>7.7234999999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>14</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.72417900000000002</v>
-      </c>
-      <c r="F11" s="1">
-        <v>39</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.30924299999999999</v>
-      </c>
-      <c r="K11" s="1">
-        <v>0.12923100000000001</v>
-      </c>
-      <c r="W11" s="1">
-        <v>7.0688000000000001E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <v>0.551616</v>
+      </c>
+      <c r="F11">
+        <v>39</v>
+      </c>
+      <c r="G11">
+        <v>0.307168</v>
+      </c>
+      <c r="K11">
+        <v>0.105889</v>
+      </c>
+      <c r="T11">
+        <v>-5.1982E-2</v>
+      </c>
+      <c r="U11">
+        <v>7.1898000000000004E-2</v>
+      </c>
+      <c r="W11">
+        <v>7.7096999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12">
-        <v>0.69864599999999999</v>
-      </c>
-      <c r="F12">
-        <v>39</v>
-      </c>
-      <c r="G12">
-        <v>0.265737</v>
-      </c>
-      <c r="K12">
-        <v>0.15495500000000001</v>
-      </c>
-      <c r="W12">
-        <v>7.4968999999999994E-2</v>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.70253500000000002</v>
+      </c>
+      <c r="F12" s="1">
+        <v>39</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.26140099999999999</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.15115000000000001</v>
+      </c>
+      <c r="W12" s="1">
+        <v>7.6502000000000001E-2</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
@@ -1387,25 +1405,25 @@
         <v>25</v>
       </c>
       <c r="E13">
-        <v>0.68267100000000003</v>
+        <v>0.69608400000000004</v>
       </c>
       <c r="F13">
         <v>39</v>
       </c>
       <c r="G13">
-        <v>0.27997100000000003</v>
+        <v>0.27523900000000001</v>
       </c>
       <c r="K13">
-        <v>0.19290399999999999</v>
+        <v>0.19187399999999999</v>
       </c>
       <c r="N13">
-        <v>-8.7156999999999998E-2</v>
+        <v>-8.9151999999999995E-2</v>
       </c>
       <c r="V13">
-        <v>3.0984000000000001E-2</v>
+        <v>3.1869000000000001E-2</v>
       </c>
       <c r="W13">
-        <v>8.2498000000000002E-2</v>
+        <v>8.3714999999999998E-2</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -1422,34 +1440,25 @@
         <v>25</v>
       </c>
       <c r="E14">
-        <v>0.66814700000000005</v>
+        <v>0.68080799999999997</v>
       </c>
       <c r="F14">
         <v>39</v>
       </c>
       <c r="G14">
-        <v>0.41008</v>
-      </c>
-      <c r="H14">
-        <v>-8.0699000000000007E-2</v>
+        <v>0.29303499999999999</v>
       </c>
       <c r="K14">
-        <v>0.16094600000000001</v>
-      </c>
-      <c r="L14">
-        <v>0.12372900000000001</v>
+        <v>0.16778799999999999</v>
       </c>
       <c r="N14">
-        <v>-0.17277400000000001</v>
-      </c>
-      <c r="O14">
-        <v>-4.8136999999999999E-2</v>
+        <v>-9.0279999999999999E-2</v>
       </c>
       <c r="V14">
-        <v>5.1595000000000002E-2</v>
+        <v>3.4148999999999999E-2</v>
       </c>
       <c r="W14">
-        <v>8.4879999999999997E-2</v>
+        <v>8.6022000000000001E-2</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
@@ -1466,25 +1475,25 @@
         <v>25</v>
       </c>
       <c r="E15">
-        <v>0.65667600000000004</v>
+        <v>0.66119300000000003</v>
       </c>
       <c r="F15">
         <v>39</v>
       </c>
       <c r="G15">
-        <v>0.27200099999999999</v>
+        <v>0.26613700000000001</v>
       </c>
       <c r="K15">
-        <v>0.16067300000000001</v>
+        <v>0.16287299999999999</v>
       </c>
       <c r="N15">
-        <v>-8.6229E-2</v>
+        <v>-8.7664000000000006E-2</v>
       </c>
       <c r="V15">
-        <v>3.3896999999999997E-2</v>
+        <v>3.4660999999999997E-2</v>
       </c>
       <c r="W15">
-        <v>9.1609999999999997E-2</v>
+        <v>9.2135999999999996E-2</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
@@ -1501,25 +1510,34 @@
         <v>25</v>
       </c>
       <c r="E16">
-        <v>0.63070999999999999</v>
+        <v>0.47622399999999998</v>
       </c>
       <c r="F16">
         <v>39</v>
       </c>
       <c r="G16">
-        <v>0.25181100000000001</v>
+        <v>0.21832299999999999</v>
       </c>
       <c r="K16">
-        <v>0.14060400000000001</v>
+        <v>0.10591299999999999</v>
       </c>
       <c r="N16">
-        <v>-8.5401000000000005E-2</v>
-      </c>
-      <c r="V16">
-        <v>3.5108E-2</v>
+        <v>-8.2407999999999995E-2</v>
+      </c>
+      <c r="Q16">
+        <v>5.4134000000000002E-2</v>
+      </c>
+      <c r="S16">
+        <v>-8.4279000000000007E-2</v>
+      </c>
+      <c r="T16">
+        <v>-7.8883999999999996E-2</v>
+      </c>
+      <c r="U16">
+        <v>0.104491</v>
       </c>
       <c r="W16">
-        <v>0.10073799999999999</v>
+        <v>0.12875700000000001</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
@@ -1536,34 +1554,34 @@
         <v>25</v>
       </c>
       <c r="E17">
-        <v>0.48551800000000001</v>
+        <v>0.55501</v>
       </c>
       <c r="F17">
         <v>39</v>
       </c>
       <c r="G17">
-        <v>0.35271799999999998</v>
+        <v>0.32856000000000002</v>
       </c>
       <c r="H17">
-        <v>-8.5526000000000005E-2</v>
+        <v>-7.1716000000000002E-2</v>
       </c>
       <c r="K17">
-        <v>0.122849</v>
+        <v>0.12431399999999999</v>
       </c>
       <c r="L17">
-        <v>0.109665</v>
+        <v>0.104599</v>
       </c>
       <c r="N17">
-        <v>-0.15001100000000001</v>
+        <v>-0.143179</v>
       </c>
       <c r="O17">
-        <v>-4.6033999999999999E-2</v>
+        <v>-5.1430999999999998E-2</v>
       </c>
       <c r="V17">
-        <v>5.0474999999999999E-2</v>
+        <v>5.1986999999999998E-2</v>
       </c>
       <c r="W17">
-        <v>0.10489800000000001</v>
+        <v>0.10523399999999999</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
@@ -1580,28 +1598,34 @@
         <v>25</v>
       </c>
       <c r="E18">
-        <v>0.44686900000000002</v>
+        <v>0.42652499999999999</v>
       </c>
       <c r="F18">
         <v>39</v>
       </c>
       <c r="G18">
-        <v>0.27398699999999998</v>
+        <v>0.30348700000000001</v>
       </c>
       <c r="H18">
-        <v>-5.7084000000000003E-2</v>
+        <v>-7.9027E-2</v>
       </c>
       <c r="K18">
-        <v>0.120755</v>
+        <v>0.120133</v>
+      </c>
+      <c r="L18">
+        <v>8.8636000000000006E-2</v>
       </c>
       <c r="N18">
-        <v>-7.9480999999999996E-2</v>
+        <v>-0.12109200000000001</v>
+      </c>
+      <c r="O18">
+        <v>-4.7406999999999998E-2</v>
       </c>
       <c r="V18">
-        <v>3.3868000000000002E-2</v>
+        <v>4.7060999999999999E-2</v>
       </c>
       <c r="W18">
-        <v>0.116864</v>
+        <v>0.11192199999999999</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
@@ -1618,37 +1642,31 @@
         <v>25</v>
       </c>
       <c r="E19">
-        <v>0.25918999999999998</v>
+        <v>0.32867600000000002</v>
       </c>
       <c r="F19">
         <v>39</v>
       </c>
       <c r="G19">
-        <v>0.39346100000000001</v>
+        <v>0.34312399999999998</v>
       </c>
       <c r="H19">
-        <v>-0.100816</v>
+        <v>-6.9306000000000006E-2</v>
       </c>
       <c r="J19">
-        <v>-4.9931999999999997E-2</v>
+        <v>-5.3372000000000003E-2</v>
       </c>
       <c r="K19">
-        <v>0.12531200000000001</v>
-      </c>
-      <c r="L19">
-        <v>9.1190999999999994E-2</v>
+        <v>0.15027199999999999</v>
       </c>
       <c r="N19">
-        <v>-0.128359</v>
-      </c>
-      <c r="O19">
-        <v>-4.6338999999999998E-2</v>
+        <v>-8.7372000000000005E-2</v>
       </c>
       <c r="V19">
-        <v>5.0076000000000002E-2</v>
+        <v>3.9421999999999999E-2</v>
       </c>
       <c r="W19">
-        <v>0.119112</v>
+        <v>0.121161</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
@@ -1665,22 +1683,22 @@
         <v>25</v>
       </c>
       <c r="E20">
-        <v>0.54932899999999996</v>
+        <v>0.56472999999999995</v>
       </c>
       <c r="F20">
         <v>39</v>
       </c>
       <c r="G20">
-        <v>0.196406</v>
+        <v>0.192583</v>
       </c>
       <c r="O20">
-        <v>-5.7485000000000001E-2</v>
+        <v>-6.2191000000000003E-2</v>
       </c>
       <c r="V20">
-        <v>3.7305999999999999E-2</v>
+        <v>3.9399000000000003E-2</v>
       </c>
       <c r="W20">
-        <v>0.13550699999999999</v>
+        <v>0.13625200000000001</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
@@ -1697,22 +1715,22 @@
         <v>25</v>
       </c>
       <c r="E21">
-        <v>0.46960800000000003</v>
+        <v>0.55639899999999998</v>
       </c>
       <c r="F21">
         <v>39</v>
       </c>
       <c r="G21">
-        <v>0.202595</v>
+        <v>0.19950399999999999</v>
       </c>
       <c r="O21">
-        <v>-5.2254000000000002E-2</v>
+        <v>-5.747E-2</v>
       </c>
       <c r="V21">
-        <v>3.5512000000000002E-2</v>
+        <v>3.7620000000000001E-2</v>
       </c>
       <c r="W21">
-        <v>0.13556599999999999</v>
+        <v>0.136269</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
@@ -1729,22 +1747,22 @@
         <v>25</v>
       </c>
       <c r="E22">
-        <v>0.47659400000000002</v>
+        <v>0.56784800000000002</v>
       </c>
       <c r="F22">
         <v>39</v>
       </c>
       <c r="G22">
-        <v>0.20455100000000001</v>
+        <v>0.20125599999999999</v>
       </c>
       <c r="O22">
-        <v>-5.4896E-2</v>
+        <v>-6.0611999999999999E-2</v>
       </c>
       <c r="V22">
-        <v>3.6260000000000001E-2</v>
+        <v>3.8443999999999999E-2</v>
       </c>
       <c r="W22">
-        <v>0.13459599999999999</v>
+        <v>0.135405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>